<commit_message>
Arreglar errorcitos en tabla
</commit_message>
<xml_diff>
--- a/lr_table_Pascal.xlsx
+++ b/lr_table_Pascal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kary\Documents\semestre_10\compiladores\proyecto_compiladores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65207917-238D-4C4E-A89C-9BA58FFAF65E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC30F1A-F51F-4530-B178-B2A4A516D5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35389252-E298-4FD3-9A6D-794169DDE1B7}"/>
   </bookViews>
@@ -2862,15 +2862,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>31</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
-          <xdr:row>114</xdr:row>
-          <xdr:rowOff>124460</xdr:rowOff>
+          <xdr:colOff>328832</xdr:colOff>
+          <xdr:row>113</xdr:row>
+          <xdr:rowOff>173502</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>32</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>115</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:col>31</xdr:col>
+          <xdr:colOff>450752</xdr:colOff>
+          <xdr:row>114</xdr:row>
+          <xdr:rowOff>90268</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2912,15 +2912,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>32</xdr:col>
-          <xdr:colOff>502920</xdr:colOff>
-          <xdr:row>114</xdr:row>
-          <xdr:rowOff>124460</xdr:rowOff>
+          <xdr:colOff>315351</xdr:colOff>
+          <xdr:row>113</xdr:row>
+          <xdr:rowOff>173502</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>33</xdr:col>
-          <xdr:colOff>30480</xdr:colOff>
-          <xdr:row>115</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:col>32</xdr:col>
+          <xdr:colOff>437271</xdr:colOff>
+          <xdr:row>114</xdr:row>
+          <xdr:rowOff>90268</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2962,15 +2962,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>31</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
-          <xdr:row>114</xdr:row>
-          <xdr:rowOff>124460</xdr:rowOff>
+          <xdr:colOff>328832</xdr:colOff>
+          <xdr:row>113</xdr:row>
+          <xdr:rowOff>173502</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>32</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>115</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:col>31</xdr:col>
+          <xdr:colOff>450752</xdr:colOff>
+          <xdr:row>114</xdr:row>
+          <xdr:rowOff>90268</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3012,15 +3012,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>32</xdr:col>
-          <xdr:colOff>373380</xdr:colOff>
-          <xdr:row>114</xdr:row>
-          <xdr:rowOff>124460</xdr:rowOff>
+          <xdr:colOff>185811</xdr:colOff>
+          <xdr:row>113</xdr:row>
+          <xdr:rowOff>173502</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>32</xdr:col>
-          <xdr:colOff>510540</xdr:colOff>
-          <xdr:row>115</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:colOff>307731</xdr:colOff>
+          <xdr:row>114</xdr:row>
+          <xdr:rowOff>90268</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3358,13 +3358,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28C03AB-2437-4C68-A311-A2FB35DB5052}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:CR153"/>
+  <dimension ref="A1:CR149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG149" sqref="AG149"/>
+      <selection pane="bottomRight" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20455,24 +20455,6 @@
       <c r="CQ149" s="5"/>
       <c r="CR149" s="5"/>
     </row>
-    <row r="151" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="G151" s="1">
-        <f>COUNTIF(B3:AW149,"*")</f>
-        <v>839</v>
-      </c>
-    </row>
-    <row r="152" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="G152" s="1">
-        <f>COUNTIF(B3:AW140,"r*")</f>
-        <v>587</v>
-      </c>
-    </row>
-    <row r="153" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="G153" s="1">
-        <f>COUNTIF(B3:AW140,"s*")</f>
-        <v>160</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="3">
@@ -20487,102 +20469,102 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1028" r:id="rId4" name="Control 4">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>31</xdr:col>
-                <xdr:colOff>510540</xdr:colOff>
-                <xdr:row>114</xdr:row>
-                <xdr:rowOff>121920</xdr:rowOff>
+                <xdr:col>32</xdr:col>
+                <xdr:colOff>182880</xdr:colOff>
+                <xdr:row>113</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>32</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>115</xdr:row>
-                <xdr:rowOff>45720</xdr:rowOff>
+                <xdr:colOff>304800</xdr:colOff>
+                <xdr:row>114</xdr:row>
+                <xdr:rowOff>91440</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1028" r:id="rId4" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1027" r:id="rId6" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>32</xdr:col>
-                <xdr:colOff>502920</xdr:colOff>
-                <xdr:row>114</xdr:row>
-                <xdr:rowOff>121920</xdr:rowOff>
+                <xdr:col>31</xdr:col>
+                <xdr:colOff>327660</xdr:colOff>
+                <xdr:row>113</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>33</xdr:col>
-                <xdr:colOff>30480</xdr:colOff>
-                <xdr:row>115</xdr:row>
-                <xdr:rowOff>45720</xdr:rowOff>
+                <xdr:col>31</xdr:col>
+                <xdr:colOff>449580</xdr:colOff>
+                <xdr:row>114</xdr:row>
+                <xdr:rowOff>91440</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1027" r:id="rId6" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId7" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1026" r:id="rId8" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>31</xdr:col>
-                <xdr:colOff>510540</xdr:colOff>
-                <xdr:row>114</xdr:row>
-                <xdr:rowOff>121920</xdr:rowOff>
+                <xdr:col>32</xdr:col>
+                <xdr:colOff>312420</xdr:colOff>
+                <xdr:row>113</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>32</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>115</xdr:row>
-                <xdr:rowOff>45720</xdr:rowOff>
+                <xdr:colOff>434340</xdr:colOff>
+                <xdr:row>114</xdr:row>
+                <xdr:rowOff>91440</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId7" name="Control 3"/>
+        <control shapeId="1026" r:id="rId8" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId8" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId9">
+        <control shapeId="1025" r:id="rId9" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>32</xdr:col>
-                <xdr:colOff>373380</xdr:colOff>
-                <xdr:row>114</xdr:row>
-                <xdr:rowOff>121920</xdr:rowOff>
+                <xdr:col>31</xdr:col>
+                <xdr:colOff>327660</xdr:colOff>
+                <xdr:row>113</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>32</xdr:col>
-                <xdr:colOff>510540</xdr:colOff>
-                <xdr:row>115</xdr:row>
-                <xdr:rowOff>45720</xdr:rowOff>
+                <xdr:col>31</xdr:col>
+                <xdr:colOff>449580</xdr:colOff>
+                <xdr:row>114</xdr:row>
+                <xdr:rowOff>91440</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId8" name="Control 4"/>
+        <control shapeId="1025" r:id="rId9" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>